<commit_message>
Add all product cover arts and code from fix-product-images branch
</commit_message>
<xml_diff>
--- a/gameshop_enter_catalogus (2).xlsx
+++ b/gameshop_enter_catalogus (2).xlsx
@@ -1,25 +1,25 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Switch" sheetId="1" state="visible" r:id="rId1"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="3DS" sheetId="2" state="visible" r:id="rId2"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="DS" sheetId="3" state="visible" r:id="rId3"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="GBA" sheetId="4" state="visible" r:id="rId4"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="GB - GBC" sheetId="5" state="visible" r:id="rId5"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="GameCube" sheetId="6" state="visible" r:id="rId6"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="N64" sheetId="7" state="visible" r:id="rId7"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="SNES" sheetId="8" state="visible" r:id="rId8"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="NES" sheetId="9" state="visible" r:id="rId9"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Wii" sheetId="10" state="visible" r:id="rId10"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Wii U" sheetId="11" state="visible" r:id="rId11"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Spelcomputers" sheetId="12" state="visible" r:id="rId12"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Accessoires &amp; Opladers" sheetId="13" state="visible" r:id="rId13"/>
+    <sheet name="Switch" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="3DS" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet name="DS" sheetId="3" state="visible" r:id="rId3"/>
+    <sheet name="GBA" sheetId="4" state="visible" r:id="rId4"/>
+    <sheet name="GB - GBC" sheetId="5" state="visible" r:id="rId5"/>
+    <sheet name="GameCube" sheetId="6" state="visible" r:id="rId6"/>
+    <sheet name="N64" sheetId="7" state="visible" r:id="rId7"/>
+    <sheet name="SNES" sheetId="8" state="visible" r:id="rId8"/>
+    <sheet name="NES" sheetId="9" state="visible" r:id="rId9"/>
+    <sheet name="Wii" sheetId="10" state="visible" r:id="rId10"/>
+    <sheet name="Wii U" sheetId="11" state="visible" r:id="rId11"/>
+    <sheet name="Spelcomputers" sheetId="12" state="visible" r:id="rId12"/>
+    <sheet name="Accessoires &amp; Opladers" sheetId="13" state="visible" r:id="rId13"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Switch'!$A$1:$E$61</definedName>
@@ -3281,7 +3281,7 @@
       </c>
       <c r="E46" s="4" t="inlineStr">
         <is>
-          <t>https://www.google.com/search?q=Zack+&amp;+Wiki+Wii+EUR+PAL+box+art+cover&amp;tbm=isch</t>
+          <t>https://www.google.com/search?q=Zack+%26+Wiki+Wii+EUR+PAL+box+art+cover&amp;tbm=isch</t>
         </is>
       </c>
     </row>
@@ -3306,7 +3306,7 @@
       </c>
       <c r="E47" s="7" t="inlineStr">
         <is>
-          <t>https://www.google.com/search?q=Sin+&amp;+Punishment:+Star+Successor+Wii+EUR+PAL+box+art+cover&amp;tbm=isch</t>
+          <t>https://www.google.com/search?q=Sin+%26+Punishment:+Star+Successor+Wii+EUR+PAL+box+art+cover&amp;tbm=isch</t>
         </is>
       </c>
     </row>
@@ -3456,7 +3456,7 @@
       </c>
       <c r="E53" s="7" t="inlineStr">
         <is>
-          <t>https://www.google.com/search?q=Mario+&amp;+Sonic+at+the+Olympic+Games+Wii+EUR+PAL+box+art+cover&amp;tbm=isch</t>
+          <t>https://www.google.com/search?q=Mario+%26+Sonic+at+the+Olympic+Games+Wii+EUR+PAL+box+art+cover&amp;tbm=isch</t>
         </is>
       </c>
     </row>
@@ -4298,7 +4298,7 @@
       </c>
       <c r="E22" s="4" t="inlineStr">
         <is>
-          <t>https://www.google.com/search?q=Tokyo+Mirage+Sessions+#FE+Wii+U+EUR+PAL+box+art+cover&amp;tbm=isch</t>
+          <t>https://www.google.com/search?q=Tokyo+Mirage+Sessions+%23FE+Wii+U+EUR+PAL+box+art+cover&amp;tbm=isch</t>
         </is>
       </c>
     </row>
@@ -4423,7 +4423,7 @@
       </c>
       <c r="E27" s="7" t="inlineStr">
         <is>
-          <t>https://www.google.com/search?q=Mario+&amp;+Sonic+at+the+Rio+2016+Wii+U+EUR+PAL+box+art+cover&amp;tbm=isch</t>
+          <t>https://www.google.com/search?q=Mario+%26+Sonic+at+the+Rio+2016+Wii+U+EUR+PAL+box+art+cover&amp;tbm=isch</t>
         </is>
       </c>
     </row>
@@ -5173,7 +5173,7 @@
       </c>
       <c r="E57" s="7" t="inlineStr">
         <is>
-          <t>https://www.google.com/search?q=Game+&amp;+Wario+Wii+U+EUR+PAL+box+art+cover&amp;tbm=isch</t>
+          <t>https://www.google.com/search?q=Game+%26+Wario+Wii+U+EUR+PAL+box+art+cover&amp;tbm=isch</t>
         </is>
       </c>
     </row>
@@ -9381,7 +9381,7 @@
       </c>
       <c r="E42" s="4" t="inlineStr">
         <is>
-          <t>https://www.google.com/search?q=Mario+&amp;+Luigi:+Dream+Team+Bros.+3DS+EUR+PAL+box+art+cover&amp;tbm=isch</t>
+          <t>https://www.google.com/search?q=Mario+%26+Luigi:+Dream+Team+Bros.+3DS+EUR+PAL+box+art+cover&amp;tbm=isch</t>
         </is>
       </c>
     </row>
@@ -10447,7 +10447,7 @@
       </c>
       <c r="E21" s="7" t="inlineStr">
         <is>
-          <t>https://www.google.com/search?q=Mario+&amp;+Luigi:+Bowser's+Inside+Story+DS+EUR+PAL+box+art+cover&amp;tbm=isch</t>
+          <t>https://www.google.com/search?q=Mario+%26+Luigi:+Bowser's+Inside+Story+DS+EUR+PAL+box+art+cover&amp;tbm=isch</t>
         </is>
       </c>
     </row>
@@ -10472,7 +10472,7 @@
       </c>
       <c r="E22" s="4" t="inlineStr">
         <is>
-          <t>https://www.google.com/search?q=Mario+&amp;+Luigi:+Partners+in+Time+DS+EUR+PAL+box+art+cover&amp;tbm=isch</t>
+          <t>https://www.google.com/search?q=Mario+%26+Luigi:+Partners+in+Time+DS+EUR+PAL+box+art+cover&amp;tbm=isch</t>
         </is>
       </c>
     </row>
@@ -11172,7 +11172,7 @@
       </c>
       <c r="E50" s="4" t="inlineStr">
         <is>
-          <t>https://www.google.com/search?q=Mario+&amp;+Sonic+at+the+Olympic+Games+DS+EUR+PAL+box+art+cover&amp;tbm=isch</t>
+          <t>https://www.google.com/search?q=Mario+%26+Sonic+at+the+Olympic+Games+DS+EUR+PAL+box+art+cover&amp;tbm=isch</t>
         </is>
       </c>
     </row>
@@ -11864,7 +11864,7 @@
       </c>
       <c r="E13" s="7" t="inlineStr">
         <is>
-          <t>https://www.google.com/search?q=Mario+&amp;+Luigi:+Superstar+Saga+GBA+EUR+PAL+box+art+cover&amp;tbm=isch</t>
+          <t>https://www.google.com/search?q=Mario+%26+Luigi:+Superstar+Saga+GBA+EUR+PAL+box+art+cover&amp;tbm=isch</t>
         </is>
       </c>
     </row>
@@ -12089,7 +12089,7 @@
       </c>
       <c r="E22" s="4" t="inlineStr">
         <is>
-          <t>https://www.google.com/search?q=Kirby+&amp;+The+Amazing+Mirror+GBA+EUR+PAL+box+art+cover&amp;tbm=isch</t>
+          <t>https://www.google.com/search?q=Kirby+%26+The+Amazing+Mirror+GBA+EUR+PAL+box+art+cover&amp;tbm=isch</t>
         </is>
       </c>
     </row>
@@ -12264,7 +12264,7 @@
       </c>
       <c r="E29" s="7" t="inlineStr">
         <is>
-          <t>https://www.google.com/search?q=Final+Fantasy+I+&amp;+II:+Dawn+of+Souls+GBA+EUR+PAL+box+art+cover&amp;tbm=isch</t>
+          <t>https://www.google.com/search?q=Final+Fantasy+I+%26+II:+Dawn+of+Souls+GBA+EUR+PAL+box+art+cover&amp;tbm=isch</t>
         </is>
       </c>
     </row>
@@ -12564,7 +12564,7 @@
       </c>
       <c r="E41" s="7" t="inlineStr">
         <is>
-          <t>https://www.google.com/search?q=Pokemon+Pinball:+Ruby+&amp;+Sapphire+GBA+EUR+PAL+box+art+cover&amp;tbm=isch</t>
+          <t>https://www.google.com/search?q=Pokemon+Pinball:+Ruby+%26+Sapphire+GBA+EUR+PAL+box+art+cover&amp;tbm=isch</t>
         </is>
       </c>
     </row>
@@ -14480,7 +14480,7 @@
       </c>
       <c r="E54" s="4" t="inlineStr">
         <is>
-          <t>https://www.google.com/search?q=Game+&amp;+Watch+Gallery+GB+-+GBC+EUR+PAL+box+art+cover&amp;tbm=isch</t>
+          <t>https://www.google.com/search?q=Game+%26+Watch+Gallery+GB+-+GBC+EUR+PAL+box+art+cover&amp;tbm=isch</t>
         </is>
       </c>
     </row>
@@ -14505,7 +14505,7 @@
       </c>
       <c r="E55" s="7" t="inlineStr">
         <is>
-          <t>https://www.google.com/search?q=Game+&amp;+Watch+Gallery+2+GB+-+GBC+EUR+PAL+box+art+cover&amp;tbm=isch</t>
+          <t>https://www.google.com/search?q=Game+%26+Watch+Gallery+2+GB+-+GBC+EUR+PAL+box+art+cover&amp;tbm=isch</t>
         </is>
       </c>
     </row>
@@ -14530,7 +14530,7 @@
       </c>
       <c r="E56" s="4" t="inlineStr">
         <is>
-          <t>https://www.google.com/search?q=Game+&amp;+Watch+Gallery+3+GB+-+GBC+EUR+PAL+box+art+cover&amp;tbm=isch</t>
+          <t>https://www.google.com/search?q=Game+%26+Watch+Gallery+3+GB+-+GBC+EUR+PAL+box+art+cover&amp;tbm=isch</t>
         </is>
       </c>
     </row>
@@ -15547,7 +15547,7 @@
       </c>
       <c r="E32" s="4" t="inlineStr">
         <is>
-          <t>https://www.google.com/search?q=Phantasy+Star+Online+Episode+I+&amp;+II+GameCube+EUR+PAL+box+art+cover&amp;tbm=isch</t>
+          <t>https://www.google.com/search?q=Phantasy+Star+Online+Episode+I+%26+II+GameCube+EUR+PAL+box+art+cover&amp;tbm=isch</t>
         </is>
       </c>
     </row>
@@ -15647,7 +15647,7 @@
       </c>
       <c r="E36" s="4" t="inlineStr">
         <is>
-          <t>https://www.google.com/search?q=Beyond+Good+&amp;+Evil+GameCube+EUR+PAL+box+art+cover&amp;tbm=isch</t>
+          <t>https://www.google.com/search?q=Beyond+Good+%26+Evil+GameCube+EUR+PAL+box+art+cover&amp;tbm=isch</t>
         </is>
       </c>
     </row>
@@ -18906,7 +18906,7 @@
       </c>
       <c r="E37" s="7" t="inlineStr">
         <is>
-          <t>https://www.google.com/search?q=Tetris+&amp;+Dr.+Mario+SNES+EUR+PAL+box+art+cover&amp;tbm=isch</t>
+          <t>https://www.google.com/search?q=Tetris+%26+Dr.+Mario+SNES+EUR+PAL+box+art+cover&amp;tbm=isch</t>
         </is>
       </c>
     </row>

</xml_diff>